<commit_message>
To convert one column of an xlsx file to txt file
</commit_message>
<xml_diff>
--- a/xlsx_to_txt/example.xlsx
+++ b/xlsx_to_txt/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Pears</t>
   </si>
   <si>
-    <t xml:space="preserve">Chennai</t>
+    <t xml:space="preserve">Bangalore</t>
   </si>
   <si>
     <t xml:space="preserve">Oranges</t>
@@ -58,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,12 +143,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>